<commit_message>
Correction to uncertainty formula! + uncertainty for pseudo-DNI sensors
</commit_message>
<xml_diff>
--- a/Sensors/sensor_defaults.xlsx
+++ b/Sensors/sensor_defaults.xlsx
@@ -27,6 +27,20 @@
     <author>MHA</author>
   </authors>
   <commentList>
+    <comment ref="L18" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">Assume cosine response correction is applied</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="AC18" authorId="0">
       <text>
         <r>
@@ -100,7 +114,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="114">
   <si>
     <t xml:space="preserve">model</t>
   </si>
@@ -316,6 +330,9 @@
     <t xml:space="preserve">*</t>
   </si>
   <si>
+    <t xml:space="preserve">@(x) x &lt; 90</t>
+  </si>
+  <si>
     <t xml:space="preserve">rsi</t>
   </si>
   <si>
@@ -364,6 +381,9 @@
     <t xml:space="preserve">SPN1</t>
   </si>
   <si>
+    <t xml:space="preserve">Datasheet</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPLite</t>
   </si>
   <si>
@@ -407,9 +427,6 @@
   </si>
   <si>
     <t xml:space="preserve">CHP1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Datasheet</t>
   </si>
   <si>
     <t xml:space="preserve">CM11</t>
@@ -458,7 +475,7 @@
     <numFmt numFmtId="172" formatCode="0.00%"/>
     <numFmt numFmtId="173" formatCode="0_ "/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -522,6 +539,12 @@
     <font>
       <sz val="10"/>
       <color rgb="FFC9211E"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="134"/>
@@ -592,7 +615,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -645,7 +668,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -737,11 +760,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="171" fontId="9" fillId="0" borderId="0" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -828,7 +855,7 @@
       <selection pane="topLeft" activeCell="L33" activeCellId="0" sqref="L33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="1" width="3.71"/>
@@ -1692,7 +1719,7 @@
       </c>
       <c r="K12" s="13" t="str">
         <f aca="false">IF(list!L18="","",list!L18)</f>
-        <v/>
+        <v>@(x) x &lt; 90</v>
       </c>
       <c r="L12" s="13" t="str">
         <f aca="false">IF(list!M18="",LOWER(A12),list!M18)</f>
@@ -2138,11 +2165,11 @@
       </c>
       <c r="E21" s="10" t="n">
         <f aca="false">list!F27</f>
-        <v>0.5</v>
+        <v>3.04138126514911</v>
       </c>
       <c r="F21" s="11" t="n">
         <f aca="false">list!G27*100</f>
-        <v>9.59744236763108</v>
+        <v>10.2489023802552</v>
       </c>
       <c r="G21" s="11" t="n">
         <f aca="false">list!H27*100</f>
@@ -2150,7 +2177,7 @@
       </c>
       <c r="H21" s="12" t="n">
         <f aca="false">list!I27</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="I21" s="11" t="n">
         <f aca="false">list!J27*100</f>
@@ -2158,7 +2185,7 @@
       </c>
       <c r="J21" s="11" t="n">
         <f aca="false">list!K27*100</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K21" s="13" t="str">
         <f aca="false">IF(list!L27="","",list!L27)</f>
@@ -2196,7 +2223,7 @@
       </c>
       <c r="F22" s="11" t="n">
         <f aca="false">list!G28*100</f>
-        <v>5.87319333923207</v>
+        <v>5.61198717033459</v>
       </c>
       <c r="G22" s="11" t="n">
         <f aca="false">list!H28*100</f>
@@ -3571,11 +3598,11 @@
   </sheetPr>
   <dimension ref="A2:AF95"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B22" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T52" activeCellId="0" sqref="T52"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B4" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AA38" activeCellId="0" sqref="AA38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="4.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.1"/>
@@ -4769,9 +4796,11 @@
         <f aca="false">AE18</f>
         <v>0</v>
       </c>
-      <c r="L18" s="28"/>
+      <c r="L18" s="28" t="s">
+        <v>71</v>
+      </c>
       <c r="M18" s="28" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="N18" s="28"/>
       <c r="O18" s="29" t="n">
@@ -4816,7 +4845,7 @@
         <v>0</v>
       </c>
       <c r="AF18" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4824,7 +4853,7 @@
         <v>12</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C19" s="9" t="n">
         <v>1</v>
@@ -4860,10 +4889,10 @@
         <v>0</v>
       </c>
       <c r="L19" s="28" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="M19" s="28" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="N19" s="28"/>
       <c r="O19" s="29" t="n">
@@ -4908,7 +4937,7 @@
         <v>0</v>
       </c>
       <c r="AF19" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4916,7 +4945,7 @@
         <v>13</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C20" s="9" t="n">
         <v>0</v>
@@ -5012,7 +5041,7 @@
         <v>14</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C21" s="9" t="n">
         <v>0</v>
@@ -5108,7 +5137,7 @@
         <v>15</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C22" s="9" t="n">
         <v>1</v>
@@ -5187,7 +5216,7 @@
         <v>0</v>
       </c>
       <c r="AF22" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5195,7 +5224,7 @@
         <v>16</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C23" s="9" t="n">
         <v>1</v>
@@ -5274,7 +5303,7 @@
         <v>0</v>
       </c>
       <c r="AF23" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5282,7 +5311,7 @@
         <v>17</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C24" s="9" t="n">
         <v>1</v>
@@ -5361,7 +5390,7 @@
         <v>0</v>
       </c>
       <c r="AF24" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5369,7 +5398,7 @@
         <v>18</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C25" s="9" t="n">
         <v>1</v>
@@ -5406,7 +5435,7 @@
       </c>
       <c r="L25" s="28"/>
       <c r="M25" s="28" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="N25" s="28"/>
       <c r="O25" s="29" t="n">
@@ -5450,7 +5479,7 @@
         <v>0</v>
       </c>
       <c r="AF25" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5458,7 +5487,7 @@
         <v>19</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C26" s="9" t="n">
         <v>1</v>
@@ -5495,7 +5524,7 @@
       </c>
       <c r="L26" s="28"/>
       <c r="M26" s="28" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="N26" s="28"/>
       <c r="O26" s="29" t="n">
@@ -5539,7 +5568,7 @@
         <v>0</v>
       </c>
       <c r="AF26" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5547,7 +5576,7 @@
         <v>20</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C27" s="9" t="n">
         <v>1</v>
@@ -5560,11 +5589,11 @@
       </c>
       <c r="F27" s="10" t="n">
         <f aca="false">SQRT(SUMSQ(S27:V27))</f>
-        <v>0.5</v>
+        <v>3.04138126514911</v>
       </c>
       <c r="G27" s="14" t="n">
         <f aca="false">SQRT(SUMSQ(W27:AA27))</f>
-        <v>0.0959744236763108</v>
+        <v>0.102489023802552</v>
       </c>
       <c r="H27" s="15" t="n">
         <f aca="false">AD27/50</f>
@@ -5572,7 +5601,7 @@
       </c>
       <c r="I27" s="10" t="n">
         <f aca="false">AC27</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="J27" s="15" t="n">
         <f aca="false">AB27</f>
@@ -5580,53 +5609,56 @@
       </c>
       <c r="K27" s="14" t="n">
         <f aca="false">AE27</f>
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="L27" s="28"/>
       <c r="M27" s="28"/>
       <c r="N27" s="28"/>
       <c r="O27" s="29" t="n">
         <f aca="false">IF(C27=1,SQRT(SUMSQ(F27,G27*H$4,H$4*K$4*H27*ABS(25-K$3),J27*H$2*COS(K$2*PI()/180),H$2*AC27/1000*SIN(K$2*PI()/180)/SIN(80*PI()/180),K$5*K27*H$4)),"")</f>
-        <v>74.5685868469979</v>
+        <v>80.3707257376392</v>
       </c>
       <c r="P27" s="29" t="n">
         <f aca="false">IF(D27=1,SQRT(SUMSQ(F27/H$3,G27,K$4*H27*ABS(25-K$3),K$5*K27))*H$3,"")</f>
-        <v>19.2013957825987</v>
+        <v>20.7222103068181</v>
       </c>
       <c r="Q27" s="29" t="str">
         <f aca="false">IF(E27=1,SQRT(SUMSQ(F27/H$2,G27,K$4*H27*ABS(25-K$3),I27:K27))*H$2,"")</f>
         <v/>
       </c>
       <c r="R27" s="30"/>
+      <c r="S27" s="9" t="n">
+        <v>3</v>
+      </c>
       <c r="U27" s="34" t="n">
         <v>0.5</v>
       </c>
       <c r="W27" s="14" t="n">
-        <v>0.0953</v>
+        <v>0.02</v>
       </c>
       <c r="X27" s="14" t="n">
         <v>0.002</v>
       </c>
       <c r="Y27" s="14" t="n">
-        <v>0.005</v>
+        <v>0.01</v>
       </c>
       <c r="Z27" s="14" t="n">
-        <v>0.01</v>
+        <v>0.1</v>
       </c>
       <c r="AB27" s="14" t="n">
         <v>0.0223606797749979</v>
       </c>
-      <c r="AC27" s="35" t="n">
-        <v>0</v>
+      <c r="AC27" s="36" t="n">
+        <v>20</v>
       </c>
       <c r="AD27" s="14" t="n">
         <v>0.01</v>
       </c>
       <c r="AE27" s="14" t="n">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="AF27" s="3" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5634,7 +5666,7 @@
         <v>21</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C28" s="9" t="n">
         <v>1</v>
@@ -5651,7 +5683,7 @@
       </c>
       <c r="G28" s="14" t="n">
         <f aca="false">SQRT(SUMSQ(W28:AA28))</f>
-        <v>0.0587319333923207</v>
+        <v>0.0561198717033459</v>
       </c>
       <c r="H28" s="15" t="n">
         <f aca="false">AD28/50</f>
@@ -5671,16 +5703,16 @@
       </c>
       <c r="L28" s="28"/>
       <c r="M28" s="28" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="N28" s="28"/>
       <c r="O28" s="29" t="n">
         <f aca="false">IF(C28=1,SQRT(SUMSQ(F28,G28*H$4,H$4*K$4*H28*ABS(25-K$3),J28*H$2*COS(K$2*PI()/180),H$2*AC28/1000*SIN(K$2*PI()/180)/SIN(80*PI()/180),K$5*K28*H$4)),"")</f>
-        <v>46.7179577132259</v>
+        <v>44.7960413641747</v>
       </c>
       <c r="P28" s="29" t="n">
         <f aca="false">IF(D28=1,SQRT(SUMSQ(F28/H$3,G28,K$4*H28*ABS(25-K$3),K$5*K28))*H$3,"")</f>
-        <v>11.7570234328252</v>
+        <v>11.235105695987</v>
       </c>
       <c r="Q28" s="29" t="str">
         <f aca="false">IF(E28=1,SQRT(SUMSQ(F28/H$2,G28,K$4*H28*ABS(25-K$3),I28:K28))*H$2,"")</f>
@@ -5694,7 +5726,7 @@
         <v>0.0212</v>
       </c>
       <c r="X28" s="14" t="n">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="Y28" s="14" t="n">
         <v>0.01</v>
@@ -5715,7 +5747,7 @@
         <v>0</v>
       </c>
       <c r="AF28" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5723,7 +5755,7 @@
         <v>22</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C29" s="9" t="n">
         <v>1</v>
@@ -5760,7 +5792,7 @@
       </c>
       <c r="L29" s="28"/>
       <c r="M29" s="28" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="N29" s="28"/>
       <c r="O29" s="29" t="n">
@@ -5804,7 +5836,7 @@
         <v>0</v>
       </c>
       <c r="AF29" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5812,7 +5844,7 @@
         <v>23</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C30" s="9" t="n">
         <v>0</v>
@@ -5891,7 +5923,7 @@
         <v>0</v>
       </c>
       <c r="AF30" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5899,7 +5931,7 @@
         <v>24</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C31" s="9" t="n">
         <v>0</v>
@@ -5936,7 +5968,7 @@
       </c>
       <c r="L31" s="28"/>
       <c r="M31" s="28" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="N31" s="28"/>
       <c r="O31" s="29" t="str">
@@ -5980,7 +6012,7 @@
         <v>0</v>
       </c>
       <c r="AF31" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5988,7 +6020,7 @@
         <v>25</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C32" s="9" t="n">
         <v>0</v>
@@ -6025,7 +6057,7 @@
       </c>
       <c r="L32" s="28"/>
       <c r="M32" s="28" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="N32" s="28"/>
       <c r="O32" s="29" t="str">
@@ -6069,7 +6101,7 @@
         <v>0</v>
       </c>
       <c r="AF32" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6077,7 +6109,7 @@
         <v>26</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C33" s="9" t="n">
         <v>1</v>
@@ -6114,7 +6146,7 @@
       </c>
       <c r="L33" s="28"/>
       <c r="M33" s="28" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="N33" s="28"/>
       <c r="O33" s="29" t="n">
@@ -6158,7 +6190,7 @@
         <v>0</v>
       </c>
       <c r="AF33" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6166,7 +6198,7 @@
         <v>27</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C34" s="9" t="n">
         <v>1</v>
@@ -6202,7 +6234,7 @@
         <v>0.02</v>
       </c>
       <c r="M34" s="28" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="O34" s="29" t="n">
         <f aca="false">IF(C34=1,SQRT(SUMSQ(F34,G34*H$4,H$4*K$4*H34*ABS(25-K$3),J34*H$2*COS(K$2*PI()/180),H$2*AC34/1000*SIN(K$2*PI()/180)/SIN(80*PI()/180),K$5*K34*H$4)),"")</f>
@@ -6244,7 +6276,7 @@
         <v>0.02</v>
       </c>
       <c r="AF34" s="3" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6252,7 +6284,7 @@
         <v>28</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C35" s="9" t="n">
         <v>0</v>
@@ -6311,7 +6343,7 @@
         <v>0.5</v>
       </c>
       <c r="V35" s="31"/>
-      <c r="W35" s="36" t="n">
+      <c r="W35" s="37" t="n">
         <v>0.008</v>
       </c>
       <c r="X35" s="14" t="n">
@@ -6324,7 +6356,7 @@
         <v>0</v>
       </c>
       <c r="AA35" s="31"/>
-      <c r="AB35" s="36" t="n">
+      <c r="AB35" s="37" t="n">
         <v>0.005</v>
       </c>
       <c r="AC35" s="9" t="n">
@@ -6337,7 +6369,7 @@
         <v>0</v>
       </c>
       <c r="AF35" s="3" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6345,7 +6377,7 @@
         <v>29</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C36" s="9" t="n">
         <v>1</v>
@@ -6431,7 +6463,7 @@
         <v>0.0025</v>
       </c>
       <c r="AF36" s="3" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6465,8 +6497,8 @@
       <c r="AE37" s="14"/>
     </row>
     <row r="38" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B38" s="37" t="s">
-        <v>104</v>
+      <c r="B38" s="38" t="s">
+        <v>105</v>
       </c>
       <c r="C38" s="9"/>
       <c r="D38" s="9"/>
@@ -8234,14 +8266,14 @@
       <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="15.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="4" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8249,7 +8281,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8257,7 +8289,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8265,7 +8297,7 @@
         <v>4</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8273,7 +8305,7 @@
         <v>5</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8281,7 +8313,7 @@
         <v>6</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8289,7 +8321,7 @@
         <v>7</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8297,7 +8329,7 @@
         <v>8</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>